<commit_message>
Fix minor things in the helper
</commit_message>
<xml_diff>
--- a/HelperTFG.xlsx
+++ b/HelperTFG.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Discos RAID" sheetId="1" r:id="rId1"/>
     <sheet name="Desorden" sheetId="2" r:id="rId2"/>
     <sheet name="Rates" sheetId="4" r:id="rId3"/>
-    <sheet name="Cicclos" sheetId="3" r:id="rId4"/>
+    <sheet name="Ciclos" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="52">
   <si>
     <t>Coste total</t>
   </si>
@@ -165,6 +165,24 @@
   </si>
   <si>
     <t>Preamble</t>
+  </si>
+  <si>
+    <t>Calculator</t>
+  </si>
+  <si>
+    <t>Bytes / packet</t>
+  </si>
+  <si>
+    <t>10 GbE Mpps</t>
+  </si>
+  <si>
+    <t>40 GbE Mpps</t>
+  </si>
+  <si>
+    <t>Speed (Gbps)</t>
+  </si>
+  <si>
+    <t>Tasa 40 GbE</t>
   </si>
 </sst>
 </file>
@@ -228,6 +246,7 @@
     <xf numFmtId="10" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" textRotation="255"/>
     </xf>
@@ -237,7 +256,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -518,7 +536,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
@@ -754,37 +772,37 @@
       <c r="B3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="11">
+      <c r="C3" s="12">
         <v>64</v>
       </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11">
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12">
         <v>100</v>
       </c>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11">
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12">
         <v>300</v>
       </c>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="11">
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12">
         <v>600</v>
       </c>
-      <c r="P3" s="11"/>
-      <c r="Q3" s="11"/>
-      <c r="R3" s="11"/>
-      <c r="S3" s="11"/>
-      <c r="T3" s="11"/>
-      <c r="U3" s="11"/>
-      <c r="V3" s="11"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="12"/>
+      <c r="R3" s="12"/>
+      <c r="S3" s="12"/>
+      <c r="T3" s="12"/>
+      <c r="U3" s="12"/>
+      <c r="V3" s="12"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="10" t="s">
         <v>21</v>
       </c>
       <c r="B4" t="s">
@@ -846,7 +864,7 @@
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A5" s="9"/>
+      <c r="A5" s="10"/>
       <c r="B5">
         <v>1</v>
       </c>
@@ -920,7 +938,7 @@
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A6" s="9"/>
+      <c r="A6" s="10"/>
       <c r="B6">
         <v>5</v>
       </c>
@@ -994,7 +1012,7 @@
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A7" s="9"/>
+      <c r="A7" s="10"/>
       <c r="B7">
         <v>10</v>
       </c>
@@ -1066,7 +1084,7 @@
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A8" s="9"/>
+      <c r="A8" s="10"/>
       <c r="B8">
         <v>15</v>
       </c>
@@ -1138,7 +1156,7 @@
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A9" s="9"/>
+      <c r="A9" s="10"/>
       <c r="B9">
         <v>20</v>
       </c>
@@ -1208,7 +1226,7 @@
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A10" s="9"/>
+      <c r="A10" s="10"/>
       <c r="B10">
         <v>25</v>
       </c>
@@ -1278,7 +1296,7 @@
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A11" s="9"/>
+      <c r="A11" s="10"/>
       <c r="B11">
         <v>30</v>
       </c>
@@ -1367,35 +1385,35 @@
       <c r="B14" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="11">
+      <c r="C14" s="12">
         <v>64</v>
       </c>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11">
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12">
         <v>100</v>
       </c>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="11">
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12">
         <v>300</v>
       </c>
-      <c r="L14" s="11"/>
-      <c r="M14" s="11"/>
-      <c r="N14" s="11"/>
-      <c r="O14" s="11">
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="12">
         <v>600</v>
       </c>
-      <c r="P14" s="11"/>
-      <c r="Q14" s="11"/>
-      <c r="R14" s="11"/>
-      <c r="S14" s="11"/>
-      <c r="T14" s="11"/>
+      <c r="P14" s="12"/>
+      <c r="Q14" s="12"/>
+      <c r="R14" s="12"/>
+      <c r="S14" s="12"/>
+      <c r="T14" s="12"/>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="11" t="s">
         <v>22</v>
       </c>
       <c r="B15" t="s">
@@ -1457,7 +1475,7 @@
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A16" s="10"/>
+      <c r="A16" s="11"/>
       <c r="B16">
         <v>1</v>
       </c>
@@ -1531,7 +1549,7 @@
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A17" s="10"/>
+      <c r="A17" s="11"/>
       <c r="B17">
         <v>5</v>
       </c>
@@ -1605,7 +1623,7 @@
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A18" s="10"/>
+      <c r="A18" s="11"/>
       <c r="B18">
         <v>10</v>
       </c>
@@ -1677,7 +1695,7 @@
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A19" s="10"/>
+      <c r="A19" s="11"/>
       <c r="B19">
         <v>15</v>
       </c>
@@ -1749,7 +1767,7 @@
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A20" s="10"/>
+      <c r="A20" s="11"/>
       <c r="B20">
         <v>20</v>
       </c>
@@ -1819,7 +1837,7 @@
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A21" s="10"/>
+      <c r="A21" s="11"/>
       <c r="B21">
         <v>25</v>
       </c>
@@ -1889,7 +1907,7 @@
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A22" s="10"/>
+      <c r="A22" s="11"/>
       <c r="B22">
         <v>30</v>
       </c>
@@ -1982,15 +2000,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J25"/>
+  <dimension ref="A2:T25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="9" max="9" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="11.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>39</v>
       </c>
@@ -2006,8 +2029,11 @@
       <c r="F2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="I2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>10</v>
       </c>
@@ -2024,8 +2050,20 @@
         <f>C3+D3+E3</f>
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="I3" t="s">
+        <v>50</v>
+      </c>
+      <c r="J3" t="s">
+        <v>47</v>
+      </c>
+      <c r="K3" t="s">
+        <v>48</v>
+      </c>
+      <c r="L3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>40</v>
       </c>
@@ -2042,8 +2080,22 @@
         <f>C4+D4+E4</f>
         <v>24</v>
       </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>10</v>
+      </c>
+      <c r="K4" s="9">
+        <f>1000 * (I4 / 8) / ($F$3 +J4)</f>
+        <v>3.6764705882352939</v>
+      </c>
+      <c r="L4" s="9">
+        <f>1000 * (I4 / 8) / ($F$4 +J4)</f>
+        <v>3.6764705882352939</v>
+      </c>
+    </row>
+    <row r="9" spans="2:20" x14ac:dyDescent="0.2">
       <c r="C9">
         <v>64</v>
       </c>
@@ -2068,378 +2120,698 @@
       <c r="J9">
         <v>1514</v>
       </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="M9">
+        <v>64</v>
+      </c>
+      <c r="N9">
+        <v>80</v>
+      </c>
+      <c r="O9">
+        <v>100</v>
+      </c>
+      <c r="P9">
+        <v>200</v>
+      </c>
+      <c r="Q9">
+        <v>300</v>
+      </c>
+      <c r="R9">
+        <v>600</v>
+      </c>
+      <c r="S9">
+        <v>1000</v>
+      </c>
+      <c r="T9">
+        <v>1514</v>
+      </c>
+    </row>
+    <row r="10" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B10">
         <v>1</v>
       </c>
-      <c r="C10" s="12">
-        <f>1000 * ($B10 / 8) / ($F$3 + C$9)</f>
+      <c r="C10" s="9">
+        <f t="shared" ref="C10:J19" si="0">1000 * ($B10 / 8) / ($F$3 + C$9)</f>
         <v>1.4204545454545454</v>
       </c>
-      <c r="D10" s="12">
-        <f>1000 * ($B10 / 8) / ($F$3 + D$9)</f>
+      <c r="D10" s="9">
+        <f t="shared" si="0"/>
         <v>1.2019230769230769</v>
       </c>
-      <c r="E10" s="12">
-        <f>1000 * ($B10 / 8) / ($F$3 + E$9)</f>
+      <c r="E10" s="9">
+        <f t="shared" si="0"/>
         <v>1.0080645161290323</v>
       </c>
-      <c r="F10" s="12">
-        <f>1000 * ($B10 / 8) / ($F$3 + F$9)</f>
+      <c r="F10" s="9">
+        <f t="shared" si="0"/>
         <v>0.5580357142857143</v>
       </c>
-      <c r="G10" s="12">
-        <f>1000 * ($B10 / 8) / ($F$3 + G$9)</f>
+      <c r="G10" s="9">
+        <f t="shared" si="0"/>
         <v>0.38580246913580246</v>
       </c>
-      <c r="H10" s="12">
-        <f>1000 * ($B10 / 8) / ($F$3 + H$9)</f>
+      <c r="H10" s="9">
+        <f t="shared" si="0"/>
         <v>0.20032051282051283</v>
       </c>
-      <c r="I10" s="12">
-        <f>1000 * ($B10 / 8) / ($F$3 + I$9)</f>
+      <c r="I10" s="9">
+        <f t="shared" si="0"/>
         <v>0.1220703125</v>
       </c>
-      <c r="J10" s="12">
-        <f>1000 * ($B10 / 8) / ($F$3 + J$9)</f>
+      <c r="J10" s="9">
+        <f t="shared" si="0"/>
         <v>8.1274382314694402E-2</v>
       </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="L10">
+        <v>5</v>
+      </c>
+      <c r="M10" s="9">
+        <f>1000 * ($L10 / 8) / ($F$4 + M$9)</f>
+        <v>7.1022727272727275</v>
+      </c>
+      <c r="N10" s="9">
+        <f t="shared" ref="N10:T17" si="1">1000 * ($L10 / 8) / ($F$4 + N$9)</f>
+        <v>6.009615384615385</v>
+      </c>
+      <c r="O10" s="9">
+        <f t="shared" si="1"/>
+        <v>5.040322580645161</v>
+      </c>
+      <c r="P10" s="9">
+        <f t="shared" si="1"/>
+        <v>2.7901785714285716</v>
+      </c>
+      <c r="Q10" s="9">
+        <f t="shared" si="1"/>
+        <v>1.9290123456790123</v>
+      </c>
+      <c r="R10" s="9">
+        <f t="shared" si="1"/>
+        <v>1.0016025641025641</v>
+      </c>
+      <c r="S10" s="9">
+        <f t="shared" si="1"/>
+        <v>0.6103515625</v>
+      </c>
+      <c r="T10" s="9">
+        <f t="shared" si="1"/>
+        <v>0.40637191157347202</v>
+      </c>
+    </row>
+    <row r="11" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B11">
         <v>2</v>
       </c>
-      <c r="C11" s="12">
-        <f>1000 * ($B11 / 8) / ($F$3 + C$9)</f>
+      <c r="C11" s="9">
+        <f t="shared" si="0"/>
         <v>2.8409090909090908</v>
       </c>
-      <c r="D11" s="12">
-        <f>1000 * ($B11 / 8) / ($F$3 + D$9)</f>
+      <c r="D11" s="9">
+        <f t="shared" si="0"/>
         <v>2.4038461538461537</v>
       </c>
-      <c r="E11" s="12">
-        <f>1000 * ($B11 / 8) / ($F$3 + E$9)</f>
+      <c r="E11" s="9">
+        <f t="shared" si="0"/>
         <v>2.0161290322580645</v>
       </c>
-      <c r="F11" s="12">
-        <f>1000 * ($B11 / 8) / ($F$3 + F$9)</f>
+      <c r="F11" s="9">
+        <f t="shared" si="0"/>
         <v>1.1160714285714286</v>
       </c>
-      <c r="G11" s="12">
-        <f>1000 * ($B11 / 8) / ($F$3 + G$9)</f>
+      <c r="G11" s="9">
+        <f t="shared" si="0"/>
         <v>0.77160493827160492</v>
       </c>
-      <c r="H11" s="12">
-        <f>1000 * ($B11 / 8) / ($F$3 + H$9)</f>
+      <c r="H11" s="9">
+        <f t="shared" si="0"/>
         <v>0.40064102564102566</v>
       </c>
-      <c r="I11" s="12">
-        <f>1000 * ($B11 / 8) / ($F$3 + I$9)</f>
+      <c r="I11" s="9">
+        <f t="shared" si="0"/>
         <v>0.244140625</v>
       </c>
-      <c r="J11" s="12">
-        <f>1000 * ($B11 / 8) / ($F$3 + J$9)</f>
+      <c r="J11" s="9">
+        <f t="shared" si="0"/>
         <v>0.1625487646293888</v>
       </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="L11">
+        <v>10</v>
+      </c>
+      <c r="M11" s="9">
+        <f t="shared" ref="M11:M17" si="2">1000 * ($L11 / 8) / ($F$4 + M$9)</f>
+        <v>14.204545454545455</v>
+      </c>
+      <c r="N11" s="9">
+        <f t="shared" si="1"/>
+        <v>12.01923076923077</v>
+      </c>
+      <c r="O11" s="9">
+        <f t="shared" si="1"/>
+        <v>10.080645161290322</v>
+      </c>
+      <c r="P11" s="9">
+        <f t="shared" si="1"/>
+        <v>5.5803571428571432</v>
+      </c>
+      <c r="Q11" s="9">
+        <f t="shared" si="1"/>
+        <v>3.8580246913580245</v>
+      </c>
+      <c r="R11" s="9">
+        <f t="shared" si="1"/>
+        <v>2.0032051282051282</v>
+      </c>
+      <c r="S11" s="9">
+        <f t="shared" si="1"/>
+        <v>1.220703125</v>
+      </c>
+      <c r="T11" s="9">
+        <f t="shared" si="1"/>
+        <v>0.81274382314694404</v>
+      </c>
+    </row>
+    <row r="12" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B12">
         <v>3</v>
       </c>
-      <c r="C12" s="12">
-        <f>1000 * ($B12 / 8) / ($F$3 + C$9)</f>
+      <c r="C12" s="9">
+        <f t="shared" si="0"/>
         <v>4.2613636363636367</v>
       </c>
-      <c r="D12" s="12">
-        <f>1000 * ($B12 / 8) / ($F$3 + D$9)</f>
+      <c r="D12" s="9">
+        <f t="shared" si="0"/>
         <v>3.6057692307692308</v>
       </c>
-      <c r="E12" s="12">
-        <f>1000 * ($B12 / 8) / ($F$3 + E$9)</f>
+      <c r="E12" s="9">
+        <f t="shared" si="0"/>
         <v>3.024193548387097</v>
       </c>
-      <c r="F12" s="12">
-        <f>1000 * ($B12 / 8) / ($F$3 + F$9)</f>
+      <c r="F12" s="9">
+        <f t="shared" si="0"/>
         <v>1.6741071428571428</v>
       </c>
-      <c r="G12" s="12">
-        <f>1000 * ($B12 / 8) / ($F$3 + G$9)</f>
+      <c r="G12" s="9">
+        <f t="shared" si="0"/>
         <v>1.1574074074074074</v>
       </c>
-      <c r="H12" s="12">
-        <f>1000 * ($B12 / 8) / ($F$3 + H$9)</f>
+      <c r="H12" s="9">
+        <f t="shared" si="0"/>
         <v>0.60096153846153844</v>
       </c>
-      <c r="I12" s="12">
-        <f>1000 * ($B12 / 8) / ($F$3 + I$9)</f>
+      <c r="I12" s="9">
+        <f t="shared" si="0"/>
         <v>0.3662109375</v>
       </c>
-      <c r="J12" s="12">
-        <f>1000 * ($B12 / 8) / ($F$3 + J$9)</f>
+      <c r="J12" s="9">
+        <f t="shared" si="0"/>
         <v>0.24382314694408322</v>
       </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="L12">
+        <v>15</v>
+      </c>
+      <c r="M12" s="9">
+        <f t="shared" si="2"/>
+        <v>21.306818181818183</v>
+      </c>
+      <c r="N12" s="9">
+        <f t="shared" si="1"/>
+        <v>18.028846153846153</v>
+      </c>
+      <c r="O12" s="9">
+        <f t="shared" si="1"/>
+        <v>15.120967741935484</v>
+      </c>
+      <c r="P12" s="9">
+        <f t="shared" si="1"/>
+        <v>8.3705357142857135</v>
+      </c>
+      <c r="Q12" s="9">
+        <f t="shared" si="1"/>
+        <v>5.7870370370370372</v>
+      </c>
+      <c r="R12" s="9">
+        <f t="shared" si="1"/>
+        <v>3.0048076923076925</v>
+      </c>
+      <c r="S12" s="9">
+        <f t="shared" si="1"/>
+        <v>1.8310546875</v>
+      </c>
+      <c r="T12" s="9">
+        <f t="shared" si="1"/>
+        <v>1.2191157347204162</v>
+      </c>
+    </row>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B13">
         <v>4</v>
       </c>
-      <c r="C13" s="12">
-        <f>1000 * ($B13 / 8) / ($F$3 + C$9)</f>
+      <c r="C13" s="9">
+        <f t="shared" si="0"/>
         <v>5.6818181818181817</v>
       </c>
-      <c r="D13" s="12">
-        <f>1000 * ($B13 / 8) / ($F$3 + D$9)</f>
+      <c r="D13" s="9">
+        <f t="shared" si="0"/>
         <v>4.8076923076923075</v>
       </c>
-      <c r="E13" s="12">
-        <f>1000 * ($B13 / 8) / ($F$3 + E$9)</f>
+      <c r="E13" s="9">
+        <f t="shared" si="0"/>
         <v>4.032258064516129</v>
       </c>
-      <c r="F13" s="12">
-        <f>1000 * ($B13 / 8) / ($F$3 + F$9)</f>
+      <c r="F13" s="9">
+        <f t="shared" si="0"/>
         <v>2.2321428571428572</v>
       </c>
-      <c r="G13" s="12">
-        <f>1000 * ($B13 / 8) / ($F$3 + G$9)</f>
+      <c r="G13" s="9">
+        <f t="shared" si="0"/>
         <v>1.5432098765432098</v>
       </c>
-      <c r="H13" s="12">
-        <f>1000 * ($B13 / 8) / ($F$3 + H$9)</f>
+      <c r="H13" s="9">
+        <f t="shared" si="0"/>
         <v>0.80128205128205132</v>
       </c>
-      <c r="I13" s="12">
-        <f>1000 * ($B13 / 8) / ($F$3 + I$9)</f>
+      <c r="I13" s="9">
+        <f t="shared" si="0"/>
         <v>0.48828125</v>
       </c>
-      <c r="J13" s="12">
-        <f>1000 * ($B13 / 8) / ($F$3 + J$9)</f>
+      <c r="J13" s="9">
+        <f t="shared" si="0"/>
         <v>0.32509752925877761</v>
       </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="L13">
+        <v>20</v>
+      </c>
+      <c r="M13" s="9">
+        <f t="shared" si="2"/>
+        <v>28.40909090909091</v>
+      </c>
+      <c r="N13" s="9">
+        <f t="shared" si="1"/>
+        <v>24.03846153846154</v>
+      </c>
+      <c r="O13" s="9">
+        <f t="shared" si="1"/>
+        <v>20.161290322580644</v>
+      </c>
+      <c r="P13" s="9">
+        <f t="shared" si="1"/>
+        <v>11.160714285714286</v>
+      </c>
+      <c r="Q13" s="9">
+        <f t="shared" si="1"/>
+        <v>7.716049382716049</v>
+      </c>
+      <c r="R13" s="9">
+        <f t="shared" si="1"/>
+        <v>4.0064102564102564</v>
+      </c>
+      <c r="S13" s="9">
+        <f t="shared" si="1"/>
+        <v>2.44140625</v>
+      </c>
+      <c r="T13" s="9">
+        <f t="shared" si="1"/>
+        <v>1.6254876462938881</v>
+      </c>
+    </row>
+    <row r="14" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B14">
         <v>5</v>
       </c>
-      <c r="C14" s="12">
-        <f>1000 * ($B14 / 8) / ($F$3 + C$9)</f>
+      <c r="C14" s="9">
+        <f t="shared" si="0"/>
         <v>7.1022727272727275</v>
       </c>
-      <c r="D14" s="12">
-        <f>1000 * ($B14 / 8) / ($F$3 + D$9)</f>
+      <c r="D14" s="9">
+        <f t="shared" si="0"/>
         <v>6.009615384615385</v>
       </c>
-      <c r="E14" s="12">
-        <f>1000 * ($B14 / 8) / ($F$3 + E$9)</f>
+      <c r="E14" s="9">
+        <f t="shared" si="0"/>
         <v>5.040322580645161</v>
       </c>
-      <c r="F14" s="12">
-        <f>1000 * ($B14 / 8) / ($F$3 + F$9)</f>
+      <c r="F14" s="9">
+        <f t="shared" si="0"/>
         <v>2.7901785714285716</v>
       </c>
-      <c r="G14" s="12">
-        <f>1000 * ($B14 / 8) / ($F$3 + G$9)</f>
+      <c r="G14" s="9">
+        <f t="shared" si="0"/>
         <v>1.9290123456790123</v>
       </c>
-      <c r="H14" s="12">
-        <f>1000 * ($B14 / 8) / ($F$3 + H$9)</f>
+      <c r="H14" s="9">
+        <f t="shared" si="0"/>
         <v>1.0016025641025641</v>
       </c>
-      <c r="I14" s="12">
-        <f>1000 * ($B14 / 8) / ($F$3 + I$9)</f>
+      <c r="I14" s="9">
+        <f t="shared" si="0"/>
         <v>0.6103515625</v>
       </c>
-      <c r="J14" s="12">
-        <f>1000 * ($B14 / 8) / ($F$3 + J$9)</f>
+      <c r="J14" s="9">
+        <f t="shared" si="0"/>
         <v>0.40637191157347202</v>
       </c>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="L14">
+        <v>25</v>
+      </c>
+      <c r="M14" s="9">
+        <f t="shared" si="2"/>
+        <v>35.511363636363633</v>
+      </c>
+      <c r="N14" s="9">
+        <f t="shared" si="1"/>
+        <v>30.048076923076923</v>
+      </c>
+      <c r="O14" s="9">
+        <f t="shared" si="1"/>
+        <v>25.201612903225808</v>
+      </c>
+      <c r="P14" s="9">
+        <f t="shared" si="1"/>
+        <v>13.950892857142858</v>
+      </c>
+      <c r="Q14" s="9">
+        <f t="shared" si="1"/>
+        <v>9.6450617283950617</v>
+      </c>
+      <c r="R14" s="9">
+        <f t="shared" si="1"/>
+        <v>5.0080128205128203</v>
+      </c>
+      <c r="S14" s="9">
+        <f t="shared" si="1"/>
+        <v>3.0517578125</v>
+      </c>
+      <c r="T14" s="9">
+        <f t="shared" si="1"/>
+        <v>2.0318595578673602</v>
+      </c>
+    </row>
+    <row r="15" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B15">
         <v>6</v>
       </c>
-      <c r="C15" s="12">
-        <f>1000 * ($B15 / 8) / ($F$3 + C$9)</f>
+      <c r="C15" s="9">
+        <f t="shared" si="0"/>
         <v>8.5227272727272734</v>
       </c>
-      <c r="D15" s="12">
-        <f>1000 * ($B15 / 8) / ($F$3 + D$9)</f>
+      <c r="D15" s="9">
+        <f t="shared" si="0"/>
         <v>7.2115384615384617</v>
       </c>
-      <c r="E15" s="12">
-        <f>1000 * ($B15 / 8) / ($F$3 + E$9)</f>
+      <c r="E15" s="9">
+        <f t="shared" si="0"/>
         <v>6.0483870967741939</v>
       </c>
-      <c r="F15" s="12">
-        <f>1000 * ($B15 / 8) / ($F$3 + F$9)</f>
+      <c r="F15" s="9">
+        <f t="shared" si="0"/>
         <v>3.3482142857142856</v>
       </c>
-      <c r="G15" s="12">
-        <f>1000 * ($B15 / 8) / ($F$3 + G$9)</f>
+      <c r="G15" s="9">
+        <f t="shared" si="0"/>
         <v>2.3148148148148149</v>
       </c>
-      <c r="H15" s="12">
-        <f>1000 * ($B15 / 8) / ($F$3 + H$9)</f>
+      <c r="H15" s="9">
+        <f t="shared" si="0"/>
         <v>1.2019230769230769</v>
       </c>
-      <c r="I15" s="12">
-        <f>1000 * ($B15 / 8) / ($F$3 + I$9)</f>
+      <c r="I15" s="9">
+        <f t="shared" si="0"/>
         <v>0.732421875</v>
       </c>
-      <c r="J15" s="12">
-        <f>1000 * ($B15 / 8) / ($F$3 + J$9)</f>
+      <c r="J15" s="9">
+        <f t="shared" si="0"/>
         <v>0.48764629388816644</v>
       </c>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="L15">
+        <v>30</v>
+      </c>
+      <c r="M15" s="9">
+        <f t="shared" si="2"/>
+        <v>42.613636363636367</v>
+      </c>
+      <c r="N15" s="9">
+        <f t="shared" si="1"/>
+        <v>36.057692307692307</v>
+      </c>
+      <c r="O15" s="9">
+        <f t="shared" si="1"/>
+        <v>30.241935483870968</v>
+      </c>
+      <c r="P15" s="9">
+        <f t="shared" si="1"/>
+        <v>16.741071428571427</v>
+      </c>
+      <c r="Q15" s="9">
+        <f t="shared" si="1"/>
+        <v>11.574074074074074</v>
+      </c>
+      <c r="R15" s="9">
+        <f t="shared" si="1"/>
+        <v>6.009615384615385</v>
+      </c>
+      <c r="S15" s="9">
+        <f t="shared" si="1"/>
+        <v>3.662109375</v>
+      </c>
+      <c r="T15" s="9">
+        <f t="shared" si="1"/>
+        <v>2.4382314694408325</v>
+      </c>
+    </row>
+    <row r="16" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B16">
         <v>7</v>
       </c>
-      <c r="C16" s="12">
-        <f>1000 * ($B16 / 8) / ($F$3 + C$9)</f>
+      <c r="C16" s="9">
+        <f t="shared" si="0"/>
         <v>9.9431818181818183</v>
       </c>
-      <c r="D16" s="12">
-        <f>1000 * ($B16 / 8) / ($F$3 + D$9)</f>
+      <c r="D16" s="9">
+        <f t="shared" si="0"/>
         <v>8.4134615384615383</v>
       </c>
-      <c r="E16" s="12">
-        <f>1000 * ($B16 / 8) / ($F$3 + E$9)</f>
+      <c r="E16" s="9">
+        <f t="shared" si="0"/>
         <v>7.056451612903226</v>
       </c>
-      <c r="F16" s="12">
-        <f>1000 * ($B16 / 8) / ($F$3 + F$9)</f>
+      <c r="F16" s="9">
+        <f t="shared" si="0"/>
         <v>3.90625</v>
       </c>
-      <c r="G16" s="12">
-        <f>1000 * ($B16 / 8) / ($F$3 + G$9)</f>
+      <c r="G16" s="9">
+        <f t="shared" si="0"/>
         <v>2.7006172839506171</v>
       </c>
-      <c r="H16" s="12">
-        <f>1000 * ($B16 / 8) / ($F$3 + H$9)</f>
+      <c r="H16" s="9">
+        <f t="shared" si="0"/>
         <v>1.4022435897435896</v>
       </c>
-      <c r="I16" s="12">
-        <f>1000 * ($B16 / 8) / ($F$3 + I$9)</f>
+      <c r="I16" s="9">
+        <f t="shared" si="0"/>
         <v>0.8544921875</v>
       </c>
-      <c r="J16" s="12">
-        <f>1000 * ($B16 / 8) / ($F$3 + J$9)</f>
+      <c r="J16" s="9">
+        <f t="shared" si="0"/>
         <v>0.56892067620286091</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L16">
+        <v>35</v>
+      </c>
+      <c r="M16" s="9">
+        <f t="shared" si="2"/>
+        <v>49.715909090909093</v>
+      </c>
+      <c r="N16" s="9">
+        <f t="shared" si="1"/>
+        <v>42.067307692307693</v>
+      </c>
+      <c r="O16" s="9">
+        <f t="shared" si="1"/>
+        <v>35.282258064516128</v>
+      </c>
+      <c r="P16" s="9">
+        <f t="shared" si="1"/>
+        <v>19.53125</v>
+      </c>
+      <c r="Q16" s="9">
+        <f t="shared" si="1"/>
+        <v>13.503086419753087</v>
+      </c>
+      <c r="R16" s="9">
+        <f t="shared" si="1"/>
+        <v>7.0112179487179489</v>
+      </c>
+      <c r="S16" s="9">
+        <f t="shared" si="1"/>
+        <v>4.2724609375</v>
+      </c>
+      <c r="T16" s="9">
+        <f t="shared" si="1"/>
+        <v>2.8446033810143043</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B17">
         <v>8</v>
       </c>
-      <c r="C17" s="12">
-        <f>1000 * ($B17 / 8) / ($F$3 + C$9)</f>
+      <c r="C17" s="9">
+        <f t="shared" si="0"/>
         <v>11.363636363636363</v>
       </c>
-      <c r="D17" s="12">
-        <f>1000 * ($B17 / 8) / ($F$3 + D$9)</f>
+      <c r="D17" s="9">
+        <f t="shared" si="0"/>
         <v>9.615384615384615</v>
       </c>
-      <c r="E17" s="12">
-        <f>1000 * ($B17 / 8) / ($F$3 + E$9)</f>
+      <c r="E17" s="9">
+        <f t="shared" si="0"/>
         <v>8.064516129032258</v>
       </c>
-      <c r="F17" s="12">
-        <f>1000 * ($B17 / 8) / ($F$3 + F$9)</f>
+      <c r="F17" s="9">
+        <f t="shared" si="0"/>
         <v>4.4642857142857144</v>
       </c>
-      <c r="G17" s="12">
-        <f>1000 * ($B17 / 8) / ($F$3 + G$9)</f>
+      <c r="G17" s="9">
+        <f t="shared" si="0"/>
         <v>3.0864197530864197</v>
       </c>
-      <c r="H17" s="12">
-        <f>1000 * ($B17 / 8) / ($F$3 + H$9)</f>
+      <c r="H17" s="9">
+        <f t="shared" si="0"/>
         <v>1.6025641025641026</v>
       </c>
-      <c r="I17" s="12">
-        <f>1000 * ($B17 / 8) / ($F$3 + I$9)</f>
+      <c r="I17" s="9">
+        <f t="shared" si="0"/>
         <v>0.9765625</v>
       </c>
-      <c r="J17" s="12">
-        <f>1000 * ($B17 / 8) / ($F$3 + J$9)</f>
+      <c r="J17" s="9">
+        <f t="shared" si="0"/>
         <v>0.65019505851755521</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L17">
+        <v>40</v>
+      </c>
+      <c r="M17" s="9">
+        <f t="shared" si="2"/>
+        <v>56.81818181818182</v>
+      </c>
+      <c r="N17" s="9">
+        <f t="shared" si="1"/>
+        <v>48.07692307692308</v>
+      </c>
+      <c r="O17" s="9">
+        <f t="shared" si="1"/>
+        <v>40.322580645161288</v>
+      </c>
+      <c r="P17" s="9">
+        <f t="shared" si="1"/>
+        <v>22.321428571428573</v>
+      </c>
+      <c r="Q17" s="9">
+        <f t="shared" si="1"/>
+        <v>15.432098765432098</v>
+      </c>
+      <c r="R17" s="9">
+        <f t="shared" si="1"/>
+        <v>8.0128205128205128</v>
+      </c>
+      <c r="S17" s="9">
+        <f t="shared" si="1"/>
+        <v>4.8828125</v>
+      </c>
+      <c r="T17" s="9">
+        <f t="shared" si="1"/>
+        <v>3.2509752925877762</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B18">
         <v>9</v>
       </c>
-      <c r="C18" s="12">
-        <f>1000 * ($B18 / 8) / ($F$3 + C$9)</f>
+      <c r="C18" s="9">
+        <f t="shared" si="0"/>
         <v>12.784090909090908</v>
       </c>
-      <c r="D18" s="12">
-        <f>1000 * ($B18 / 8) / ($F$3 + D$9)</f>
+      <c r="D18" s="9">
+        <f t="shared" si="0"/>
         <v>10.817307692307692</v>
       </c>
-      <c r="E18" s="12">
-        <f>1000 * ($B18 / 8) / ($F$3 + E$9)</f>
+      <c r="E18" s="9">
+        <f t="shared" si="0"/>
         <v>9.07258064516129</v>
       </c>
-      <c r="F18" s="12">
-        <f>1000 * ($B18 / 8) / ($F$3 + F$9)</f>
+      <c r="F18" s="9">
+        <f t="shared" si="0"/>
         <v>5.0223214285714288</v>
       </c>
-      <c r="G18" s="12">
-        <f>1000 * ($B18 / 8) / ($F$3 + G$9)</f>
+      <c r="G18" s="9">
+        <f t="shared" si="0"/>
         <v>3.4722222222222223</v>
       </c>
-      <c r="H18" s="12">
-        <f>1000 * ($B18 / 8) / ($F$3 + H$9)</f>
+      <c r="H18" s="9">
+        <f t="shared" si="0"/>
         <v>1.8028846153846154</v>
       </c>
-      <c r="I18" s="12">
-        <f>1000 * ($B18 / 8) / ($F$3 + I$9)</f>
+      <c r="I18" s="9">
+        <f t="shared" si="0"/>
         <v>1.0986328125</v>
       </c>
-      <c r="J18" s="12">
-        <f>1000 * ($B18 / 8) / ($F$3 + J$9)</f>
+      <c r="J18" s="9">
+        <f t="shared" si="0"/>
         <v>0.73146944083224963</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="9"/>
+      <c r="P18" s="9"/>
+      <c r="Q18" s="9"/>
+      <c r="R18" s="9"/>
+      <c r="S18" s="9"/>
+      <c r="T18" s="9"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B19">
         <v>10</v>
       </c>
-      <c r="C19" s="12">
-        <f>1000 * ($B19 / 8) / ($F$3 + C$9)</f>
+      <c r="C19" s="9">
+        <f t="shared" si="0"/>
         <v>14.204545454545455</v>
       </c>
-      <c r="D19" s="12">
-        <f>1000 * ($B19 / 8) / ($F$3 + D$9)</f>
+      <c r="D19" s="9">
+        <f t="shared" si="0"/>
         <v>12.01923076923077</v>
       </c>
-      <c r="E19" s="12">
-        <f>1000 * ($B19 / 8) / ($F$3 + E$9)</f>
+      <c r="E19" s="9">
+        <f t="shared" si="0"/>
         <v>10.080645161290322</v>
       </c>
-      <c r="F19" s="12">
-        <f>1000 * ($B19 / 8) / ($F$3 + F$9)</f>
+      <c r="F19" s="9">
+        <f t="shared" si="0"/>
         <v>5.5803571428571432</v>
       </c>
-      <c r="G19" s="12">
-        <f>1000 * ($B19 / 8) / ($F$3 + G$9)</f>
+      <c r="G19" s="9">
+        <f t="shared" si="0"/>
         <v>3.8580246913580245</v>
       </c>
-      <c r="H19" s="12">
-        <f>1000 * ($B19 / 8) / ($F$3 + H$9)</f>
+      <c r="H19" s="9">
+        <f t="shared" si="0"/>
         <v>2.0032051282051282</v>
       </c>
-      <c r="I19" s="12">
-        <f>1000 * ($B19 / 8) / ($F$3 + I$9)</f>
+      <c r="I19" s="9">
+        <f t="shared" si="0"/>
         <v>1.220703125</v>
       </c>
-      <c r="J19" s="12">
-        <f>1000 * ($B19 / 8) / ($F$3 + J$9)</f>
+      <c r="J19" s="9">
+        <f t="shared" si="0"/>
         <v>0.81274382314694404</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="9"/>
+      <c r="R19" s="9"/>
+      <c r="S19" s="9"/>
+      <c r="T19" s="9"/>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>43</v>
       </c>
@@ -2468,7 +2840,7 @@
         <v>1514</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>10</v>
       </c>
@@ -2480,68 +2852,71 @@
         <v>7.2727272727272725</v>
       </c>
       <c r="D24" s="7">
-        <f t="shared" ref="D24:J25" si="0" xml:space="preserve"> $A24 * D$23/ (D$23 + $F3)</f>
+        <f t="shared" ref="D24:J25" si="3" xml:space="preserve"> $A24 * D$23/ (D$23 + $F3)</f>
         <v>7.6923076923076925</v>
       </c>
       <c r="E24" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>8.064516129032258</v>
       </c>
       <c r="F24" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>8.9285714285714288</v>
       </c>
       <c r="G24" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>9.2592592592592595</v>
       </c>
       <c r="H24" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>9.615384615384615</v>
       </c>
       <c r="I24" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>9.765625</v>
       </c>
       <c r="J24" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>9.8439531859557867</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>40</v>
+      </c>
+      <c r="B25" t="s">
+        <v>51</v>
       </c>
       <c r="C25" s="7">
         <f xml:space="preserve"> $A25 * C$23/ (C$23 + $F4)</f>
         <v>29.09090909090909</v>
       </c>
       <c r="D25" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>30.76923076923077</v>
       </c>
       <c r="E25" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>32.258064516129032</v>
       </c>
       <c r="F25" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>35.714285714285715</v>
       </c>
       <c r="G25" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>37.037037037037038</v>
       </c>
       <c r="H25" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>38.46153846153846</v>
       </c>
       <c r="I25" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>39.0625</v>
       </c>
       <c r="J25" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>39.375812743823147</v>
       </c>
     </row>
@@ -2579,10 +2954,10 @@
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="11"/>
+      <c r="F5" s="12"/>
       <c r="I5" t="s">
         <v>32</v>
       </c>

</xml_diff>